<commit_message>
Added GDP and URB data, adapted parameter parsing to format version 0.2.
</commit_message>
<xml_diff>
--- a/RECC_Classifications_Master_V10.xlsx
+++ b/RECC_Classifications_Master_V10.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="19"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover_Dimensions_Aspects" sheetId="8" r:id="rId1"/>
@@ -3590,7 +3590,7 @@
   <dimension ref="B4:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6687,11 +6687,11 @@
   </sheetPr>
   <dimension ref="A1:AW1311"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomRight" activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20917,7 +20917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -21364,7 +21364,7 @@
   </sheetPr>
   <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>

</xml_diff>